<commit_message>
Sides for bias test and final test are random now
But needs to be saved in cdv
</commit_message>
<xml_diff>
--- a/to_do.xlsx
+++ b/to_do.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">TO DO </t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>add 1 more noun training</t>
+  </si>
+  <si>
+    <t>maybe give every row a unique number in addition to 1-8 for all conditions</t>
   </si>
 </sst>
 </file>
@@ -423,7 +426,7 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -476,6 +479,11 @@
     <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1">

</xml_diff>